<commit_message>
added connection to SSRS
</commit_message>
<xml_diff>
--- a/temp1.xlsx
+++ b/temp1.xlsx
@@ -2837,7 +2837,7 @@
         <v>0.0</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>100.0</v>
+        <v>56.0</v>
       </c>
       <c r="D4" s="25" t="str">
         <f ref="D4:D35" si="0" t="shared">IF(AND(C4&lt;=H4,C4&gt;=I4),"PASS","FAIL")</f>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="E4" s="11" t="n">
         <f>(C4-B4)</f>
-        <v>100.0</v>
+        <v>56.0</v>
       </c>
       <c r="F4" s="26" t="e">
         <f>E4/B4</f>
@@ -2989,7 +2989,7 @@
         <v>0.0</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>100.0</v>
+        <v>156.0441</v>
       </c>
       <c r="D8" s="25" t="str">
         <f si="0" t="shared"/>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="E8" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>156.0441</v>
       </c>
       <c r="F8" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3028,7 +3028,7 @@
         <v>0.0</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>100.0</v>
+        <v>124.3936</v>
       </c>
       <c r="D9" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="E9" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>124.3936</v>
       </c>
       <c r="F9" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3067,7 +3067,7 @@
         <v>0.0</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>100.0</v>
+        <v>123.3568</v>
       </c>
       <c r="D10" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="E10" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>123.3568</v>
       </c>
       <c r="F10" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3106,7 +3106,7 @@
         <v>0.0</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>100.0</v>
+        <v>135.9624</v>
       </c>
       <c r="D11" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E11" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>135.9624</v>
       </c>
       <c r="F11" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3223,7 +3223,7 @@
         <v>0.0</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>100.0</v>
+        <v>127.5859</v>
       </c>
       <c r="D14" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="E14" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>127.5859</v>
       </c>
       <c r="F14" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3262,7 +3262,7 @@
         <v>0.0</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>100.0</v>
+        <v>104.6938</v>
       </c>
       <c r="D15" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="E15" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>104.6938</v>
       </c>
       <c r="F15" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3301,7 +3301,7 @@
         <v>0.0</v>
       </c>
       <c r="C16" s="5" t="n">
-        <v>100.0</v>
+        <v>137.9815</v>
       </c>
       <c r="D16" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="E16" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>137.9815</v>
       </c>
       <c r="F16" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3340,7 +3340,7 @@
         <v>0.0</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>100.0</v>
+        <v>145.9214</v>
       </c>
       <c r="D17" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="E17" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>145.9214</v>
       </c>
       <c r="F17" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3379,7 +3379,7 @@
         <v>0.0</v>
       </c>
       <c r="C18" s="5" t="n">
-        <v>100.0</v>
+        <v>152.961</v>
       </c>
       <c r="D18" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="E18" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>152.961</v>
       </c>
       <c r="F18" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3418,7 +3418,7 @@
         <v>0.0</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>100.0</v>
+        <v>141.2284</v>
       </c>
       <c r="D19" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="E19" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>141.2284</v>
       </c>
       <c r="F19" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3457,7 +3457,7 @@
         <v>0.0</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>100.0</v>
+        <v>156.9991</v>
       </c>
       <c r="D20" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="E20" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>156.9991</v>
       </c>
       <c r="F20" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3496,7 +3496,7 @@
         <v>0.0</v>
       </c>
       <c r="C21" s="5" t="n">
-        <v>100.0</v>
+        <v>141.8833</v>
       </c>
       <c r="D21" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3504,7 +3504,7 @@
       </c>
       <c r="E21" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>141.8833</v>
       </c>
       <c r="F21" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3535,7 +3535,7 @@
         <v>0.0</v>
       </c>
       <c r="C22" s="5" t="n">
-        <v>100.0</v>
+        <v>138.2271</v>
       </c>
       <c r="D22" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3543,7 +3543,7 @@
       </c>
       <c r="E22" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>138.2271</v>
       </c>
       <c r="F22" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3574,7 +3574,7 @@
         <v>0.0</v>
       </c>
       <c r="C23" s="5" t="n">
-        <v>100.0</v>
+        <v>166.9309</v>
       </c>
       <c r="D23" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="E23" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>166.9309</v>
       </c>
       <c r="F23" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3613,7 +3613,7 @@
         <v>0.0</v>
       </c>
       <c r="C24" s="5" t="n">
-        <v>100.0</v>
+        <v>143.4385</v>
       </c>
       <c r="D24" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="E24" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>143.4385</v>
       </c>
       <c r="F24" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3652,7 +3652,7 @@
         <v>0.0</v>
       </c>
       <c r="C25" s="5" t="n">
-        <v>100.0</v>
+        <v>127.4767</v>
       </c>
       <c r="D25" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3660,7 +3660,7 @@
       </c>
       <c r="E25" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>127.4767</v>
       </c>
       <c r="F25" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3691,7 +3691,7 @@
         <v>0.0</v>
       </c>
       <c r="C26" s="5" t="n">
-        <v>100.0</v>
+        <v>135.4986</v>
       </c>
       <c r="D26" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="E26" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>135.4986</v>
       </c>
       <c r="F26" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3730,7 +3730,7 @@
         <v>0.0</v>
       </c>
       <c r="C27" s="5" t="n">
-        <v>100.0</v>
+        <v>134.6254</v>
       </c>
       <c r="D27" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="E27" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>134.6254</v>
       </c>
       <c r="F27" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3769,7 +3769,7 @@
         <v>0.0</v>
       </c>
       <c r="C28" s="5" t="n">
-        <v>100.0</v>
+        <v>128.3226</v>
       </c>
       <c r="D28" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="E28" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>128.3226</v>
       </c>
       <c r="F28" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3808,7 +3808,7 @@
         <v>0.0</v>
       </c>
       <c r="C29" s="5" t="n">
-        <v>100.0</v>
+        <v>151.0783</v>
       </c>
       <c r="D29" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="E29" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>151.0783</v>
       </c>
       <c r="F29" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3847,7 +3847,7 @@
         <v>0.0</v>
       </c>
       <c r="C30" s="5" t="n">
-        <v>100.0</v>
+        <v>139.6187</v>
       </c>
       <c r="D30" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="E30" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>139.6187</v>
       </c>
       <c r="F30" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3886,7 +3886,7 @@
         <v>0.0</v>
       </c>
       <c r="C31" s="5" t="n">
-        <v>100.0</v>
+        <v>148.8682</v>
       </c>
       <c r="D31" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="E31" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>148.8682</v>
       </c>
       <c r="F31" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3925,7 +3925,7 @@
         <v>0.0</v>
       </c>
       <c r="C32" s="5" t="n">
-        <v>100.0</v>
+        <v>131.515</v>
       </c>
       <c r="D32" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="E32" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>131.515</v>
       </c>
       <c r="F32" s="26" t="e">
         <f si="4" t="shared"/>
@@ -3964,7 +3964,7 @@
         <v>0.0</v>
       </c>
       <c r="C33" s="5" t="n">
-        <v>100.0</v>
+        <v>140.9556</v>
       </c>
       <c r="D33" s="25" t="str">
         <f si="0" t="shared"/>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="E33" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>140.9556</v>
       </c>
       <c r="F33" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4003,7 +4003,7 @@
         <v>0.0</v>
       </c>
       <c r="C34" s="5" t="n">
-        <v>100.0</v>
+        <v>107.4496</v>
       </c>
       <c r="D34" s="25" t="str">
         <f si="0" t="shared"/>
@@ -4011,7 +4011,7 @@
       </c>
       <c r="E34" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>107.4496</v>
       </c>
       <c r="F34" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4042,7 +4042,7 @@
         <v>0.0</v>
       </c>
       <c r="C35" s="5" t="n">
-        <v>100.0</v>
+        <v>147.2311</v>
       </c>
       <c r="D35" s="25" t="str">
         <f si="0" t="shared"/>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="E35" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>147.2311</v>
       </c>
       <c r="F35" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4081,7 +4081,7 @@
         <v>0.0</v>
       </c>
       <c r="C36" s="5" t="n">
-        <v>100.0</v>
+        <v>150.9965</v>
       </c>
       <c r="D36" s="25" t="str">
         <f ref="D36:D67" si="5" t="shared">IF(AND(C36&lt;=H36,C36&gt;=I36),"PASS","FAIL")</f>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="E36" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>150.9965</v>
       </c>
       <c r="F36" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4120,7 +4120,7 @@
         <v>0.0</v>
       </c>
       <c r="C37" s="5" t="n">
-        <v>100.0</v>
+        <v>123.2749</v>
       </c>
       <c r="D37" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="E37" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>123.2749</v>
       </c>
       <c r="F37" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4159,7 +4159,7 @@
         <v>0.0</v>
       </c>
       <c r="C38" s="5" t="n">
-        <v>100.0</v>
+        <v>185.1845</v>
       </c>
       <c r="D38" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="E38" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>185.1845</v>
       </c>
       <c r="F38" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4198,7 +4198,7 @@
         <v>0.0</v>
       </c>
       <c r="C39" s="5" t="n">
-        <v>100.0</v>
+        <v>153.3702</v>
       </c>
       <c r="D39" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="E39" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>153.3702</v>
       </c>
       <c r="F39" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4237,7 +4237,7 @@
         <v>0.0</v>
       </c>
       <c r="C40" s="5" t="n">
-        <v>100.0</v>
+        <v>144.4208</v>
       </c>
       <c r="D40" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="E40" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>144.4208</v>
       </c>
       <c r="F40" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4277,7 +4277,7 @@
         <v>0.0</v>
       </c>
       <c r="C41" s="5" t="n">
-        <v>100.0</v>
+        <v>118.1453</v>
       </c>
       <c r="D41" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="E41" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>118.1453</v>
       </c>
       <c r="F41" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4317,7 +4317,7 @@
         <v>0.0</v>
       </c>
       <c r="C42" s="5" t="n">
-        <v>100.0</v>
+        <v>135.1166</v>
       </c>
       <c r="D42" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4325,7 +4325,7 @@
       </c>
       <c r="E42" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>135.1166</v>
       </c>
       <c r="F42" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4357,7 +4357,7 @@
         <v>0.0</v>
       </c>
       <c r="C43" s="5" t="n">
-        <v>100.0</v>
+        <v>143.4658</v>
       </c>
       <c r="D43" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="E43" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>143.4658</v>
       </c>
       <c r="F43" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4397,7 +4397,7 @@
         <v>0.0</v>
       </c>
       <c r="C44" s="5" t="n">
-        <v>100.0</v>
+        <v>134.5163</v>
       </c>
       <c r="D44" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="E44" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>134.5163</v>
       </c>
       <c r="F44" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4437,7 +4437,7 @@
         <v>0.0</v>
       </c>
       <c r="C45" s="5" t="n">
-        <v>100.0</v>
+        <v>134.2434</v>
       </c>
       <c r="D45" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="E45" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>134.2434</v>
       </c>
       <c r="F45" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4477,7 +4477,7 @@
         <v>0.0</v>
       </c>
       <c r="C46" s="5" t="n">
-        <v>100.0</v>
+        <v>170.6963</v>
       </c>
       <c r="D46" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4485,7 +4485,7 @@
       </c>
       <c r="E46" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>170.6963</v>
       </c>
       <c r="F46" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4517,7 +4517,7 @@
         <v>0.0</v>
       </c>
       <c r="C47" s="5" t="n">
-        <v>100.0</v>
+        <v>134.3799</v>
       </c>
       <c r="D47" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4525,7 +4525,7 @@
       </c>
       <c r="E47" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>134.3799</v>
       </c>
       <c r="F47" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4557,7 +4557,7 @@
         <v>0.0</v>
       </c>
       <c r="C48" s="5" t="n">
-        <v>100.0</v>
+        <v>154.1342</v>
       </c>
       <c r="D48" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="E48" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>154.1342</v>
       </c>
       <c r="F48" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4597,7 +4597,7 @@
         <v>0.0</v>
       </c>
       <c r="C49" s="5" t="n">
-        <v>100.0</v>
+        <v>155.5803</v>
       </c>
       <c r="D49" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="E49" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>155.5803</v>
       </c>
       <c r="F49" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4637,7 +4637,7 @@
         <v>0.0</v>
       </c>
       <c r="C50" s="5" t="n">
-        <v>100.0</v>
+        <v>144.5026</v>
       </c>
       <c r="D50" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="E50" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>144.5026</v>
       </c>
       <c r="F50" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4677,7 +4677,7 @@
         <v>0.0</v>
       </c>
       <c r="C51" s="5" t="n">
-        <v>100.0</v>
+        <v>142.5381</v>
       </c>
       <c r="D51" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="E51" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>142.5381</v>
       </c>
       <c r="F51" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4717,7 +4717,7 @@
         <v>0.0</v>
       </c>
       <c r="C52" s="5" t="n">
-        <v>100.0</v>
+        <v>151.9242</v>
       </c>
       <c r="D52" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="E52" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>151.9242</v>
       </c>
       <c r="F52" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4757,7 +4757,7 @@
         <v>0.0</v>
       </c>
       <c r="C53" s="5" t="n">
-        <v>100.0</v>
+        <v>149.6322</v>
       </c>
       <c r="D53" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="E53" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>149.6322</v>
       </c>
       <c r="F53" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4797,7 +4797,7 @@
         <v>0.0</v>
       </c>
       <c r="C54" s="5" t="n">
-        <v>100.0</v>
+        <v>133.9434</v>
       </c>
       <c r="D54" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4805,7 +4805,7 @@
       </c>
       <c r="E54" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>133.9434</v>
       </c>
       <c r="F54" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4837,7 +4837,7 @@
         <v>0.0</v>
       </c>
       <c r="C55" s="5" t="n">
-        <v>100.0</v>
+        <v>135.9351</v>
       </c>
       <c r="D55" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="E55" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>135.9351</v>
       </c>
       <c r="F55" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4877,7 +4877,7 @@
         <v>0.0</v>
       </c>
       <c r="C56" s="5" t="n">
-        <v>100.0</v>
+        <v>139.0183</v>
       </c>
       <c r="D56" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="E56" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>139.0183</v>
       </c>
       <c r="F56" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4915,7 +4915,7 @@
         <v>0.0</v>
       </c>
       <c r="C57" s="5" t="n">
-        <v>100.0</v>
+        <v>148.3226</v>
       </c>
       <c r="D57" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4923,7 +4923,7 @@
       </c>
       <c r="E57" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>148.3226</v>
       </c>
       <c r="F57" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4953,7 +4953,7 @@
         <v>0.0</v>
       </c>
       <c r="C58" s="5" t="n">
-        <v>100.0</v>
+        <v>140.6282</v>
       </c>
       <c r="D58" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="E58" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>140.6282</v>
       </c>
       <c r="F58" s="26" t="e">
         <f si="4" t="shared"/>
@@ -4991,7 +4991,7 @@
         <v>0.0</v>
       </c>
       <c r="C59" s="5" t="n">
-        <v>100.0</v>
+        <v>153.0974</v>
       </c>
       <c r="D59" s="25" t="str">
         <f si="5" t="shared"/>
@@ -4999,7 +4999,7 @@
       </c>
       <c r="E59" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>153.0974</v>
       </c>
       <c r="F59" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5029,7 +5029,7 @@
         <v>0.0</v>
       </c>
       <c r="C60" s="5" t="n">
-        <v>100.0</v>
+        <v>143.7932</v>
       </c>
       <c r="D60" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="E60" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>143.7932</v>
       </c>
       <c r="F60" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5067,7 +5067,7 @@
         <v>0.0</v>
       </c>
       <c r="C61" s="5" t="n">
-        <v>100.0</v>
+        <v>154.2707</v>
       </c>
       <c r="D61" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="E61" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>154.2707</v>
       </c>
       <c r="F61" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5105,7 +5105,7 @@
         <v>0.0</v>
       </c>
       <c r="C62" s="5" t="n">
-        <v>100.0</v>
+        <v>134.9801</v>
       </c>
       <c r="D62" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5113,7 +5113,7 @@
       </c>
       <c r="E62" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>134.9801</v>
       </c>
       <c r="F62" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5143,7 +5143,7 @@
         <v>0.0</v>
       </c>
       <c r="C63" s="5" t="n">
-        <v>100.0</v>
+        <v>173.2065</v>
       </c>
       <c r="D63" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="E63" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>173.2065</v>
       </c>
       <c r="F63" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5181,7 +5181,7 @@
         <v>0.0</v>
       </c>
       <c r="C64" s="5" t="n">
-        <v>100.0</v>
+        <v>148.3226</v>
       </c>
       <c r="D64" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="E64" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>148.3226</v>
       </c>
       <c r="F64" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5219,7 +5219,7 @@
         <v>0.0</v>
       </c>
       <c r="C65" s="5" t="n">
-        <v>100.0</v>
+        <v>144.6936</v>
       </c>
       <c r="D65" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="E65" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>144.6936</v>
       </c>
       <c r="F65" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5257,7 +5257,7 @@
         <v>0.0</v>
       </c>
       <c r="C66" s="5" t="n">
-        <v>100.0</v>
+        <v>176.5352</v>
       </c>
       <c r="D66" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="E66" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>176.5352</v>
       </c>
       <c r="F66" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5295,7 +5295,7 @@
         <v>0.0</v>
       </c>
       <c r="C67" s="5" t="n">
-        <v>100.0</v>
+        <v>158.0633</v>
       </c>
       <c r="D67" s="25" t="str">
         <f si="5" t="shared"/>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="E67" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>158.0633</v>
       </c>
       <c r="F67" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5333,7 +5333,7 @@
         <v>0.0</v>
       </c>
       <c r="C68" s="5" t="n">
-        <v>100.0</v>
+        <v>138.3635</v>
       </c>
       <c r="D68" s="25" t="str">
         <f ref="D68:D99" si="8" t="shared">IF(AND(C68&lt;=H68,C68&gt;=I68),"PASS","FAIL")</f>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="E68" s="11" t="n">
         <f si="3" t="shared"/>
-        <v>100.0</v>
+        <v>138.3635</v>
       </c>
       <c r="F68" s="26" t="e">
         <f si="4" t="shared"/>
@@ -5371,7 +5371,7 @@
         <v>0.0</v>
       </c>
       <c r="C69" s="5" t="n">
-        <v>100.0</v>
+        <v>154.6799</v>
       </c>
       <c r="D69" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="E69" s="11" t="n">
         <f ref="E69:E99" si="9" t="shared">(C69-B69)</f>
-        <v>100.0</v>
+        <v>154.6799</v>
       </c>
       <c r="F69" s="26" t="e">
         <f ref="F69:F99" si="10" t="shared">E69/B69</f>
@@ -5409,7 +5409,7 @@
         <v>0.0</v>
       </c>
       <c r="C70" s="5" t="n">
-        <v>100.0</v>
+        <v>141.6923</v>
       </c>
       <c r="D70" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="E70" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>141.6923</v>
       </c>
       <c r="F70" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5447,7 +5447,7 @@
         <v>0.0</v>
       </c>
       <c r="C71" s="5" t="n">
-        <v>100.0</v>
+        <v>140.1916</v>
       </c>
       <c r="D71" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5455,7 +5455,7 @@
       </c>
       <c r="E71" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>140.1916</v>
       </c>
       <c r="F71" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5485,7 +5485,7 @@
         <v>0.0</v>
       </c>
       <c r="C72" s="5" t="n">
-        <v>100.0</v>
+        <v>126.6037</v>
       </c>
       <c r="D72" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="E72" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>126.6037</v>
       </c>
       <c r="F72" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5523,7 +5523,7 @@
         <v>0.0</v>
       </c>
       <c r="C73" s="5" t="n">
-        <v>100.0</v>
+        <v>140.3826</v>
       </c>
       <c r="D73" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5531,7 +5531,7 @@
       </c>
       <c r="E73" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>140.3826</v>
       </c>
       <c r="F73" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5561,7 +5561,7 @@
         <v>0.0</v>
       </c>
       <c r="C74" s="5" t="n">
-        <v>100.0</v>
+        <v>140.0006</v>
       </c>
       <c r="D74" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5569,7 +5569,7 @@
       </c>
       <c r="E74" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>140.0006</v>
       </c>
       <c r="F74" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5599,7 +5599,7 @@
         <v>0.0</v>
       </c>
       <c r="C75" s="5" t="n">
-        <v>100.0</v>
+        <v>146.3307</v>
       </c>
       <c r="D75" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="E75" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>146.3307</v>
       </c>
       <c r="F75" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5637,7 +5637,7 @@
         <v>0.0</v>
       </c>
       <c r="C76" s="5" t="n">
-        <v>100.0</v>
+        <v>128.7046</v>
       </c>
       <c r="D76" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5645,7 +5645,7 @@
       </c>
       <c r="E76" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>128.7046</v>
       </c>
       <c r="F76" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5675,7 +5675,7 @@
         <v>0.0</v>
       </c>
       <c r="C77" s="5" t="n">
-        <v>100.0</v>
+        <v>131.133</v>
       </c>
       <c r="D77" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5683,7 +5683,7 @@
       </c>
       <c r="E77" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>131.133</v>
       </c>
       <c r="F77" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5713,7 +5713,7 @@
         <v>0.0</v>
       </c>
       <c r="C78" s="5" t="n">
-        <v>100.0</v>
+        <v>138.5</v>
       </c>
       <c r="D78" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="E78" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>138.5</v>
       </c>
       <c r="F78" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5751,7 +5751,7 @@
         <v>0.0</v>
       </c>
       <c r="C79" s="5" t="n">
-        <v>100.0</v>
+        <v>139.5913</v>
       </c>
       <c r="D79" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="E79" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>139.5913</v>
       </c>
       <c r="F79" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5789,7 +5789,7 @@
         <v>0.0</v>
       </c>
       <c r="C80" s="5" t="n">
-        <v>100.0</v>
+        <v>115.6624</v>
       </c>
       <c r="D80" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="E80" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>115.6624</v>
       </c>
       <c r="F80" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5827,7 +5827,7 @@
         <v>0.0</v>
       </c>
       <c r="C81" s="5" t="n">
-        <v>100.0</v>
+        <v>156.699</v>
       </c>
       <c r="D81" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5835,7 +5835,7 @@
       </c>
       <c r="E81" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>156.699</v>
       </c>
       <c r="F81" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5865,7 +5865,7 @@
         <v>0.0</v>
       </c>
       <c r="C82" s="5" t="n">
-        <v>100.0</v>
+        <v>144.639</v>
       </c>
       <c r="D82" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5873,7 +5873,7 @@
       </c>
       <c r="E82" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>144.639</v>
       </c>
       <c r="F82" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5903,7 +5903,7 @@
         <v>0.0</v>
       </c>
       <c r="C83" s="5" t="n">
-        <v>100.0</v>
+        <v>157.5448</v>
       </c>
       <c r="D83" s="25" t="str">
         <f si="8" t="shared"/>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="E83" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>157.5448</v>
       </c>
       <c r="F83" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5941,15 +5941,15 @@
         <v>0.0</v>
       </c>
       <c r="C84" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D84" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E84" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F84" s="26" t="e">
         <f si="10" t="shared"/>
@@ -5979,15 +5979,15 @@
         <v>0.0</v>
       </c>
       <c r="C85" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D85" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E85" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F85" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6017,15 +6017,15 @@
         <v>0.0</v>
       </c>
       <c r="C86" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D86" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E86" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F86" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6055,15 +6055,15 @@
         <v>0.0</v>
       </c>
       <c r="C87" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D87" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E87" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F87" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6093,15 +6093,15 @@
         <v>0.0</v>
       </c>
       <c r="C88" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D88" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E88" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F88" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6131,15 +6131,15 @@
         <v>0.0</v>
       </c>
       <c r="C89" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D89" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E89" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F89" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6169,15 +6169,15 @@
         <v>0.0</v>
       </c>
       <c r="C90" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D90" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E90" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F90" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6207,15 +6207,15 @@
         <v>0.0</v>
       </c>
       <c r="C91" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D91" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E91" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F91" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6245,15 +6245,15 @@
         <v>0.0</v>
       </c>
       <c r="C92" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D92" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E92" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F92" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6283,15 +6283,15 @@
         <v>0.0</v>
       </c>
       <c r="C93" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D93" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E93" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F93" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6321,15 +6321,15 @@
         <v>0.0</v>
       </c>
       <c r="C94" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D94" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E94" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F94" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6359,15 +6359,15 @@
         <v>0.0</v>
       </c>
       <c r="C95" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D95" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E95" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F95" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6397,15 +6397,15 @@
         <v>0.0</v>
       </c>
       <c r="C96" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D96" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E96" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F96" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6435,15 +6435,15 @@
         <v>0.0</v>
       </c>
       <c r="C97" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D97" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E97" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F97" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6473,15 +6473,15 @@
         <v>0.0</v>
       </c>
       <c r="C98" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D98" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E98" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F98" s="26" t="e">
         <f si="10" t="shared"/>
@@ -6511,15 +6511,15 @@
         <v>0.0</v>
       </c>
       <c r="C99" s="5" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="D99" s="25" t="str">
         <f si="8" t="shared"/>
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="E99" s="11" t="n">
         <f si="9" t="shared"/>
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="F99" s="26" t="e">
         <f si="10" t="shared"/>

</xml_diff>